<commit_message>
Added final code but not tested
</commit_message>
<xml_diff>
--- a/resources/testdata/testdata.xlsx
+++ b/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Audithya\blazedemo-portal\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3114932-7F3D-452E-8F27-21EA5A1C0485}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DB9D89-98C3-487B-BEBF-88DBE1C5ECF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,24 +25,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>TestScript</t>
   </si>
   <si>
-    <t>DepartureStation</t>
-  </si>
-  <si>
-    <t>DestinationStation</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
     <t>Address</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>CreditCardNumber</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>NameOnCard</t>
+  </si>
+  <si>
+    <t>BookAFlight</t>
+  </si>
+  <si>
+    <t>SourceCity</t>
+  </si>
+  <si>
+    <t>DestinationCity</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Sai Audithya</t>
+  </si>
+  <si>
+    <t>E9 DMV Skyland</t>
+  </si>
+  <si>
+    <t>Nellore</t>
+  </si>
+  <si>
+    <t>Andhra</t>
+  </si>
+  <si>
+    <t>1111222233334444</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>Sai Audithya S</t>
   </si>
 </sst>
 </file>
@@ -92,9 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,40 +427,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <v>524004</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>